<commit_message>
Add 05machinelearning.R which includes predictive model of covariates and separately the strategies. Strategies represented using the 75th percentile dummy variables. Add table output to report. All tables are put together as dataframes in rptnice_tables.R.
</commit_message>
<xml_diff>
--- a/output_tables.xlsx
+++ b/output_tables.xlsx
@@ -11,6 +11,8 @@
     <sheet name="tbl2" sheetId="2" r:id="rId2"/>
     <sheet name="tbl3" sheetId="3" r:id="rId3"/>
     <sheet name="tbl4" sheetId="4" r:id="rId4"/>
+    <sheet name="tbl5" sheetId="5" r:id="rId5"/>
+    <sheet name="tbl6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1548,4 +1550,304 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Construct</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Percent iterations among top 5 predictors</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SVI Overall Rank</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Percent Black or African American</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Derivedtotalenrolled</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Percent free and/or reduced lunch eligible</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Percent two or more races</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Percent American Indian/Alaska Native</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Locale</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Change in county COVID-19 case rate</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Percent Hispanic or Latino</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Percent Native Hawaiian or other Pacific Islander</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Percent White</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Percent Asian</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Percent no race specified</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Construct</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Percent iterations among top 5 predictors</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vaccination</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Testing and/or screening</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Physical distancing</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cohorting and/or staggering policy</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Etiquette</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Trace and quarantine</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Masking</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ventilation</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cleaning</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stay home</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-wrote results. analyses done for now.
</commit_message>
<xml_diff>
--- a/output_tables.xlsx
+++ b/output_tables.xlsx
@@ -1437,7 +1437,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1454,6 +1454,11 @@
           <t>Coefficient (95% interval)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1466,6 +1471,9 @@
           <t>-0.08 (-0.69, 0.53)</t>
         </is>
       </c>
+      <c r="C2">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1478,6 +1486,9 @@
           <t>-0.13 (-0.54, 0.27)</t>
         </is>
       </c>
+      <c r="C3">
+        <v>0.5600000000000001</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1490,6 +1501,9 @@
           <t>-0.38 (-0.83, 0.03)</t>
         </is>
       </c>
+      <c r="C4">
+        <v>0.07000000000000001</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1502,6 +1516,9 @@
           <t>-0.35 (-0.84, 0.2)</t>
         </is>
       </c>
+      <c r="C5">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1514,6 +1531,9 @@
           <t>-0.33 (-0.71, 0.03)</t>
         </is>
       </c>
+      <c r="C6">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1526,6 +1546,9 @@
           <t>-0.17 (-0.54, 0.22)</t>
         </is>
       </c>
+      <c r="C7">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1538,6 +1561,9 @@
           <t>-0.29 (-0.72, 0.08)</t>
         </is>
       </c>
+      <c r="C8">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1550,6 +1576,9 @@
           <t>-0.09 (-0.53, 0.31)</t>
         </is>
       </c>
+      <c r="C9">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1562,6 +1591,9 @@
           <t>0.03 (-0.98, 0.96)</t>
         </is>
       </c>
+      <c r="C10">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1573,6 +1605,9 @@
         <is>
           <t>-0.38 (-0.78, 0.02)</t>
         </is>
+      </c>
+      <c r="C11">
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1599,6 +1634,11 @@
           <t>Coefficient (95% interval)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1611,6 +1651,9 @@
           <t>1.04 (0.32, 1.78)</t>
         </is>
       </c>
+      <c r="C2">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1623,6 +1666,9 @@
           <t>0.33 (-0.44, 1.1)</t>
         </is>
       </c>
+      <c r="C3">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1635,6 +1681,9 @@
           <t>0.14 (-0.35, 0.68)</t>
         </is>
       </c>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1647,6 +1696,9 @@
           <t>-0.28 (-0.84, 0.3)</t>
         </is>
       </c>
+      <c r="C5">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1659,6 +1711,9 @@
           <t>-0.31 (-0.99, 0.36)</t>
         </is>
       </c>
+      <c r="C6">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1671,6 +1726,9 @@
           <t>-0.2 (-0.85, 0.47)</t>
         </is>
       </c>
+      <c r="C7">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1683,6 +1741,9 @@
           <t>0.13 (-0.42, 0.69)</t>
         </is>
       </c>
+      <c r="C8">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1695,6 +1756,9 @@
           <t>-0.06 (-0.7, 0.56)</t>
         </is>
       </c>
+      <c r="C9">
+        <v>0.86</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1707,6 +1771,9 @@
           <t>0.33 (-0.23, 0.82)</t>
         </is>
       </c>
+      <c r="C10">
+        <v>0.24</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1719,6 +1786,9 @@
           <t>0.25 (-0.6, 1.29)</t>
         </is>
       </c>
+      <c r="C11">
+        <v>0.62</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1731,6 +1801,9 @@
           <t>-0.4 (-1.01, 0.17)</t>
         </is>
       </c>
+      <c r="C12">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1743,6 +1816,9 @@
           <t>0.24 (0.04, 0.46)</t>
         </is>
       </c>
+      <c r="C13">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1755,6 +1831,9 @@
           <t>0.01 (-0.21, 0.23)</t>
         </is>
       </c>
+      <c r="C14">
+        <v>0.9399999999999999</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1767,6 +1846,9 @@
           <t>-0.15 (-0.5, 0.26)</t>
         </is>
       </c>
+      <c r="C15">
+        <v>0.42</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1779,6 +1861,9 @@
           <t>-0.25 (-0.57, 0.1)</t>
         </is>
       </c>
+      <c r="C16">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1791,6 +1876,9 @@
           <t>0.04 (-0.2, 0.28)</t>
         </is>
       </c>
+      <c r="C17">
+        <v>0.76</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1803,6 +1891,9 @@
           <t>-0.07 (-0.35, 0.18)</t>
         </is>
       </c>
+      <c r="C18">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1815,6 +1906,9 @@
           <t>0.31 (-0.15, 0.8)</t>
         </is>
       </c>
+      <c r="C19">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1827,6 +1921,9 @@
           <t>0.27 (-0.19, 0.72)</t>
         </is>
       </c>
+      <c r="C20">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1838,6 +1935,9 @@
         <is>
           <t>-0.08 (-0.45, 0.3)</t>
         </is>
+      </c>
+      <c r="C21">
+        <v>0.62</v>
       </c>
     </row>
   </sheetData>
@@ -1847,7 +1947,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1864,6 +1964,11 @@
           <t>Coefficient (95% interval)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1876,6 +1981,9 @@
           <t>1.07 (0.33, 1.76)</t>
         </is>
       </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1888,6 +1996,9 @@
           <t>-0.2 (-0.73, 0.31)</t>
         </is>
       </c>
+      <c r="C3">
+        <v>0.44</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1900,6 +2011,9 @@
           <t>-0.09 (-0.67, 0.39)</t>
         </is>
       </c>
+      <c r="C4">
+        <v>0.73</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1912,6 +2026,9 @@
           <t>-0.21 (-0.82, 0.36)</t>
         </is>
       </c>
+      <c r="C5">
+        <v>0.43</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1924,6 +2041,9 @@
           <t>0.25 (0.04, 0.46)</t>
         </is>
       </c>
+      <c r="C6">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1936,6 +2056,9 @@
           <t>0.01 (-0.2, 0.21)</t>
         </is>
       </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1948,6 +2071,9 @@
           <t>-0.19 (-0.52, 0.15)</t>
         </is>
       </c>
+      <c r="C8">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1960,6 +2086,9 @@
           <t>-0.28 (-0.6, 0.03)</t>
         </is>
       </c>
+      <c r="C9">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1972,6 +2101,9 @@
           <t>0.03 (-0.18, 0.26)</t>
         </is>
       </c>
+      <c r="C10">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1984,6 +2116,9 @@
           <t>-0.08 (-0.33, 0.21)</t>
         </is>
       </c>
+      <c r="C11">
+        <v>0.5600000000000001</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1996,6 +2131,9 @@
           <t>0.3 (-0.17, 0.8)</t>
         </is>
       </c>
+      <c r="C12">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2008,6 +2146,9 @@
           <t>0.27 (-0.21, 0.73)</t>
         </is>
       </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2019,6 +2160,9 @@
         <is>
           <t>-0.09 (-0.45, 0.22)</t>
         </is>
+      </c>
+      <c r="C14">
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>
@@ -2028,7 +2172,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2045,6 +2189,11 @@
           <t>Coefficient (95% interval)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2057,6 +2206,9 @@
           <t>1.02 (0.34, 1.67)</t>
         </is>
       </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2069,6 +2221,9 @@
           <t>0.15 (-0.41, 0.77)</t>
         </is>
       </c>
+      <c r="C3">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2081,6 +2236,9 @@
           <t>-0.23 (-0.79, 0.29)</t>
         </is>
       </c>
+      <c r="C4">
+        <v>0.39</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2093,6 +2251,9 @@
           <t>-0.53 (-1.07, -0.05)</t>
         </is>
       </c>
+      <c r="C5">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2105,6 +2266,9 @@
           <t>0.24 (0.03, 0.46)</t>
         </is>
       </c>
+      <c r="C6">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2117,6 +2281,9 @@
           <t>0.01 (-0.22, 0.22)</t>
         </is>
       </c>
+      <c r="C7">
+        <v>0.9399999999999999</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2129,6 +2296,9 @@
           <t>-0.19 (-0.55, 0.19)</t>
         </is>
       </c>
+      <c r="C8">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2141,6 +2311,9 @@
           <t>-0.28 (-0.58, 0.05)</t>
         </is>
       </c>
+      <c r="C9">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2153,6 +2326,9 @@
           <t>0.03 (-0.2, 0.27)</t>
         </is>
       </c>
+      <c r="C10">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2165,6 +2341,9 @@
           <t>-0.07 (-0.35, 0.16)</t>
         </is>
       </c>
+      <c r="C11">
+        <v>0.5600000000000001</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2177,6 +2356,9 @@
           <t>0.28 (-0.18, 0.74)</t>
         </is>
       </c>
+      <c r="C12">
+        <v>0.24</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2189,6 +2371,9 @@
           <t>0.24 (-0.18, 0.71)</t>
         </is>
       </c>
+      <c r="C13">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2200,6 +2385,9 @@
         <is>
           <t>-0.09 (-0.41, 0.3)</t>
         </is>
+      </c>
+      <c r="C14">
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>